<commit_message>
Add corridor support and update template
</commit_message>
<xml_diff>
--- a/public/input_template.xlsx
+++ b/public/input_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10511"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarkancicek/rack-diagram-web/public/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarkancicek/Codes/rack-diagram-web/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27566CA-AF0A-E242-A51E-A27F541DD9C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12073D14-4AFD-C147-97D4-E000320CB804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="500" windowWidth="22260" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4340" yWindow="760" windowWidth="22260" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kabin-2-1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="58">
   <si>
     <t>U</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>BX23902135</t>
+  </si>
+  <si>
+    <t>Corridor</t>
   </si>
 </sst>
 </file>
@@ -352,7 +355,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -395,37 +398,33 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -714,10 +713,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -730,7 +729,7 @@
     <col min="8" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -752,8 +751,11 @@
       <c r="G1" s="17" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -773,8 +775,11 @@
       <c r="G2" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -794,8 +799,11 @@
       <c r="G3" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -817,8 +825,11 @@
       <c r="G4" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -838,8 +849,11 @@
       <c r="G5" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -859,8 +873,11 @@
       <c r="G6" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -880,8 +897,11 @@
       <c r="G7" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -901,8 +921,11 @@
       <c r="G8" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -922,8 +945,11 @@
       <c r="G9" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -945,8 +971,11 @@
       <c r="G10" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -966,8 +995,11 @@
       <c r="G11" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -987,8 +1019,11 @@
       <c r="G12" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1008,8 +1043,11 @@
       <c r="G13" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H13" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1029,8 +1067,11 @@
       <c r="G14" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1050,8 +1091,11 @@
       <c r="G15" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1071,8 +1115,11 @@
       <c r="G16" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1091,6 +1138,9 @@
       <c r="F17" s="5"/>
       <c r="G17" s="6">
         <v>4</v>
+      </c>
+      <c r="H17" s="23">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1106,10 +1156,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FD6DE0C-2FF4-4FE4-ACA3-A334BA13FC40}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1122,7 +1172,7 @@
     <col min="8" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -1144,8 +1194,11 @@
       <c r="G1" s="17" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1165,8 +1218,11 @@
       <c r="G2" s="15" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1176,8 +1232,11 @@
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
       <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H3" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1187,8 +1246,11 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
       <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1198,8 +1260,11 @@
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="12"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1209,8 +1274,11 @@
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="12"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1220,8 +1288,11 @@
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
       <c r="G7" s="15"/>
-    </row>
-    <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H7" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1231,8 +1302,11 @@
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="15"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1242,8 +1316,11 @@
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="15"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1253,8 +1330,11 @@
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
       <c r="G10" s="15"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1264,8 +1344,11 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1275,8 +1358,11 @@
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
       <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1286,8 +1372,11 @@
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
       <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H13" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1297,8 +1386,11 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1308,8 +1400,11 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1319,8 +1414,11 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="6"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1330,8 +1428,11 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="6"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H17" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1341,8 +1442,11 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1352,6 +1456,9 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="6"/>
+      <c r="H19" s="23">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1365,300 +1472,339 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599D9C5F-C245-4552-A781-82A39306C387}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.83203125" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.33203125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="21.5" style="19" customWidth="1"/>
-    <col min="5" max="7" width="8.6640625" style="19" customWidth="1"/>
-    <col min="8" max="16384" width="9.1640625" style="19"/>
+    <col min="1" max="1" width="3.33203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.83203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.33203125" style="18" customWidth="1"/>
+    <col min="4" max="4" width="21.5" style="18" customWidth="1"/>
+    <col min="5" max="7" width="8.6640625" style="18" customWidth="1"/>
+    <col min="8" max="16384" width="9.1640625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="18" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="17" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="20">
-        <v>1</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="23" t="s">
+      <c r="H1" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="19">
+        <v>1</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="22">
         <v>39</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="20">
-        <v>2</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="22" t="s">
+      <c r="G2" s="23">
+        <v>1</v>
+      </c>
+      <c r="H2" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="19">
+        <v>2</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="24">
         <v>34</v>
       </c>
-      <c r="F3" s="26"/>
-      <c r="G3" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="20">
+      <c r="F3" s="24"/>
+      <c r="G3" s="23">
+        <v>2</v>
+      </c>
+      <c r="H3" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="19">
         <v>3</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="22" t="s">
+      <c r="B4" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="22">
         <v>32</v>
       </c>
-      <c r="F4" s="24"/>
-      <c r="G4" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="20">
+      <c r="F4" s="22"/>
+      <c r="G4" s="23">
+        <v>2</v>
+      </c>
+      <c r="H4" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="19">
         <v>4</v>
       </c>
-      <c r="B5" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="22" t="s">
+      <c r="B5" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="24">
         <v>30</v>
       </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="20">
+      <c r="F5" s="24"/>
+      <c r="G5" s="23">
+        <v>2</v>
+      </c>
+      <c r="H5" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="19">
         <v>5</v>
       </c>
-      <c r="B6" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="22" t="s">
+      <c r="B6" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="25">
         <v>28</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="20">
+      <c r="G6" s="22">
+        <v>1</v>
+      </c>
+      <c r="H6" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="19">
         <v>6</v>
       </c>
-      <c r="B7" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="26">
         <v>24</v>
       </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="20">
+      <c r="F7" s="26"/>
+      <c r="G7" s="22">
+        <v>2</v>
+      </c>
+      <c r="H7" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="19">
         <v>7</v>
       </c>
-      <c r="B8" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="22" t="s">
+      <c r="B8" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="26">
         <v>23</v>
       </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="20">
+      <c r="F8" s="26"/>
+      <c r="G8" s="22">
+        <v>1</v>
+      </c>
+      <c r="H8" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="19">
         <v>8</v>
       </c>
-      <c r="B9" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="22" t="s">
+      <c r="B9" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="26">
         <v>22</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="20">
+      <c r="G9" s="22">
+        <v>1</v>
+      </c>
+      <c r="H9" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="19">
         <v>9</v>
       </c>
-      <c r="B10" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="22" t="s">
+      <c r="B10" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D10" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="26">
         <v>20</v>
       </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="20">
-        <v>10</v>
-      </c>
-      <c r="B11" s="21" t="s">
+      <c r="F10" s="26"/>
+      <c r="G10" s="22">
+        <v>2</v>
+      </c>
+      <c r="H10" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="19">
+        <v>10</v>
+      </c>
+      <c r="B11" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E11" s="26">
         <v>17</v>
       </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="24">
+      <c r="F11" s="26"/>
+      <c r="G11" s="22">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="20">
+      <c r="H11" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="19">
         <v>11</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E12" s="26">
         <v>16</v>
       </c>
-      <c r="F12" s="28"/>
-      <c r="G12" s="24">
+      <c r="F12" s="26"/>
+      <c r="G12" s="22">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="20">
+      <c r="H12" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="19">
         <v>12</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="29">
+      <c r="E13" s="27">
         <v>12</v>
       </c>
-      <c r="F13" s="29"/>
-      <c r="G13" s="24">
+      <c r="F13" s="27"/>
+      <c r="G13" s="22">
+        <v>2</v>
+      </c>
+      <c r="H13" s="23">
         <v>2</v>
       </c>
     </row>

</xml_diff>